<commit_message>
add lr = 0.05
</commit_message>
<xml_diff>
--- a/evaluation_scores.xlsx
+++ b/evaluation_scores.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lintzuru/Documents/GitHub/Emotion_Classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B74540-2A75-0D4A-985F-BC259DF85653}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024083D6-1C14-9642-86DD-E4F00BDFBA3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15420" yWindow="860" windowWidth="28800" windowHeight="15640" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOG" sheetId="1" r:id="rId1"/>
     <sheet name="tf-idf" sheetId="2" r:id="rId2"/>
     <sheet name="Comparison" sheetId="3" r:id="rId3"/>
+    <sheet name="Count of data" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="67">
   <si>
     <t>Emotion</t>
   </si>
@@ -163,13 +164,94 @@
   </si>
   <si>
     <t>BOG_tfidf</t>
+  </si>
+  <si>
+    <t>Traning Data</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Emotion</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test Data</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Percentage</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>~=82.3%</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>~= 17.7%</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>learning rate = 0.05</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>[[ 75 127]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [ 80 864]] </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>[[102  59]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [ 60 925]] </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>[[ 49  78]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> [127 892]]</t>
+  </si>
+  <si>
+    <t>[[ 54  51]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [110 931]] </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>[[ 95  95]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [ 78 878]]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>[[ 85  80]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [ 66 915]] </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> [ 69 940]]</t>
+  </si>
+  <si>
+    <t>[[ 95  42]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -197,13 +279,32 @@
       <family val="2"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -220,7 +321,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -231,6 +332,21 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -547,14 +663,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -679,6 +796,124 @@
     <row r="15" spans="1:3">
       <c r="B15" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="8"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19">
+        <v>0.63157894736842102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="16">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21">
+        <v>0.32343234323432302</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="B22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23">
+        <v>0.40148698884758299</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="B24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25">
+        <v>0.52341597796143202</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="B26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27">
+        <v>0.537974683544303</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="B28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="16">
+      <c r="A29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29">
+        <v>0.63122923588039803</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="B30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31">
+        <v>0.42016806722688999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="B32" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -852,7 +1087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -1074,4 +1309,223 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3953C51A-8FC5-F940-B0E3-3E367803DFA6}">
+  <dimension ref="A3:J14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4">
+        <v>777</v>
+      </c>
+      <c r="C6">
+        <f>B6/B13</f>
+        <v>0.14575126617895329</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="4">
+        <v>162</v>
+      </c>
+      <c r="H6">
+        <f>G6/G13</f>
+        <v>0.14148471615720523</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="4">
+        <v>751</v>
+      </c>
+      <c r="C7">
+        <f>B7/B13</f>
+        <v>0.14087413243293942</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="4">
+        <v>164</v>
+      </c>
+      <c r="H7">
+        <f>G7/G13</f>
+        <v>0.14323144104803492</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4">
+        <v>758</v>
+      </c>
+      <c r="C8">
+        <f>B8/B13</f>
+        <v>0.14218720690302006</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="4">
+        <v>164</v>
+      </c>
+      <c r="H8">
+        <f>G8/G13</f>
+        <v>0.14323144104803492</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4">
+        <v>758</v>
+      </c>
+      <c r="C9">
+        <f>B9/B13</f>
+        <v>0.14218720690302006</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="4">
+        <v>173</v>
+      </c>
+      <c r="H9">
+        <f>G9/G13</f>
+        <v>0.15109170305676856</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="4">
+        <v>768</v>
+      </c>
+      <c r="C10">
+        <f>B10/B13</f>
+        <v>0.14406302757456388</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="4">
+        <v>155</v>
+      </c>
+      <c r="H10">
+        <f>G10/G13</f>
+        <v>0.13537117903930132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="4">
+        <v>758</v>
+      </c>
+      <c r="C11">
+        <f>B11/B13</f>
+        <v>0.14218720690302006</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="4">
+        <v>176</v>
+      </c>
+      <c r="H11">
+        <f>G11/G13</f>
+        <v>0.15371179039301311</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="4">
+        <v>761</v>
+      </c>
+      <c r="C12">
+        <f>B12/B13</f>
+        <v>0.14274995310448321</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="4">
+        <v>151</v>
+      </c>
+      <c r="H12">
+        <f>G12/G13</f>
+        <v>0.13187772925764193</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="B13">
+        <f>SUM(B6:B12)</f>
+        <v>5331</v>
+      </c>
+      <c r="G13">
+        <f>SUM(G6:G12)</f>
+        <v>1145</v>
+      </c>
+      <c r="J13">
+        <v>6476</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>